<commit_message>
added a helpful message for negative numbers
</commit_message>
<xml_diff>
--- a/CalculatorWPF/export.xlsx
+++ b/CalculatorWPF/export.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Distance</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>0 Hours, 49 Minutes</t>
+  </si>
+  <si>
+    <t>8 Hours, 34 Minutes</t>
   </si>
 </sst>
 </file>
@@ -104,8 +107,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="ExportTable" displayName="ExportTable" ref="A1:J4" headerRowCount="1">
-  <autoFilter ref="A1:J4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="ExportTable" displayName="ExportTable" ref="A1:J5" headerRowCount="1">
+  <autoFilter ref="A1:J5"/>
   <tableColumns count="10">
     <tableColumn id="1" name="Distance"/>
     <tableColumn id="2" name="Speed"/>
@@ -124,7 +127,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -258,6 +261,38 @@
         <v>140</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" s="0">
+        <v>300</v>
+      </c>
+      <c r="B5" s="0">
+        <v>35</v>
+      </c>
+      <c r="C5" s="0">
+        <v>60</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="0">
+        <v>0</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="0">
+        <v>514</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="0">
+        <v>35</v>
+      </c>
+      <c r="J5" s="0">
+        <v>300</v>
+      </c>
+    </row>
   </sheetData>
   <headerFooter/>
   <tableParts>

</xml_diff>